<commit_message>
Update burn down chart and 3rd scrum meeting.
</commit_message>
<xml_diff>
--- a/Scrum Files/Sprint 1/Sprint 1 Burn down chart.xlsx
+++ b/Scrum Files/Sprint 1/Sprint 1 Burn down chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E944E3C-E66E-4105-A434-F02CCFFC695C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE18AC-DC0D-43A0-AA5D-B4288D6FD2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Day</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Time Spent (h)</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Expected Sprint Points</t>
@@ -207,27 +204,28 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10/22/2024</c:v>
+                  <c:v>45587</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10/27/2024</c:v>
+                  <c:v>45592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10/30/2024</c:v>
+                  <c:v>45595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>TBD</c:v>
+                  <c:v>45600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11/5/2024</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>45601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -242,7 +240,10 @@
                   <c:v>21.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.75</c:v>
+                  <c:v>16.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -281,27 +282,28 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10/22/2024</c:v>
+                  <c:v>45587</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10/27/2024</c:v>
+                  <c:v>45592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10/30/2024</c:v>
+                  <c:v>45595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>TBD</c:v>
+                  <c:v>45600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11/5/2024</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>45601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -317,6 +319,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>34.119999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.286999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,27 +360,28 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10/22/2024</c:v>
+                  <c:v>45587</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10/27/2024</c:v>
+                  <c:v>45592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10/30/2024</c:v>
+                  <c:v>45595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>TBD</c:v>
+                  <c:v>45600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11/5/2024</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>45601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -420,14 +426,14 @@
         <c:axId val="1291348608"/>
         <c:axId val="1291364928"/>
       </c:lineChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="1291348608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -467,10 +473,9 @@
         <c:crossAx val="1291364928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="1291364928"/>
         <c:scaling>
@@ -1520,7 +1525,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1542,7 +1547,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1578,7 +1583,7 @@
         <v>45595</v>
       </c>
       <c r="B4">
-        <v>14.75</v>
+        <v>16.75</v>
       </c>
       <c r="C4">
         <v>34.119999999999997</v>
@@ -1588,8 +1593,14 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5" s="1">
+        <v>45600</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>49.286999999999999</v>
       </c>
       <c r="D5">
         <v>9.8000000000000007</v>

</xml_diff>

<commit_message>
Correct documents for sprint 1.
</commit_message>
<xml_diff>
--- a/Scrum Files/Sprint 1/Sprint 1 Burn down chart.xlsx
+++ b/Scrum Files/Sprint 1/Sprint 1 Burn down chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE18AC-DC0D-43A0-AA5D-B4288D6FD2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFD3677-08EF-4DF1-B78A-0A3CE53C70D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Day</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Expected Sprint Points</t>
+  </si>
+  <si>
+    <t>Product Backlog</t>
   </si>
 </sst>
 </file>
@@ -82,9 +85,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -234,16 +240,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.200000000000003</c:v>
+                  <c:v>55.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.25</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.75</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -323,6 +332,9 @@
                 <c:pt idx="3">
                   <c:v>49.286999999999999</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.286999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -350,7 +362,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -390,16 +402,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.200000000000003</c:v>
+                  <c:v>55.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.4</c:v>
+                  <c:v>35.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.600000000000001</c:v>
+                  <c:v>23.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.8000000000000007</c:v>
+                  <c:v>3.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -475,6 +487,8 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
+        <c:minorUnit val="1"/>
+        <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="1291364928"/>
@@ -608,7 +622,576 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Product Burn</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Down Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sprint Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45587</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45622</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>291.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC00-4F6F-81FD-81EE4A19E830}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time Spent (h)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45587</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45622</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$21:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.286999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CC00-4F6F-81FD-81EE4A19E830}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected Sprint Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45587</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45622</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$21:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>291.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>235.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CC00-4F6F-81FD-81EE4A19E830}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="353003264"/>
+        <c:axId val="352992704"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="353003264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352992704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="352992704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="353003264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1164,6 +1747,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1197,6 +2296,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>544512</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>187325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>522287</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7067565-73A1-290F-6EF0-EC4458378BF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1522,10 +2657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC08104-6C28-4261-A13C-09D20918E634}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1555,13 +2690,13 @@
         <v>45587</v>
       </c>
       <c r="B2">
-        <v>39.200000000000003</v>
+        <v>55.2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>39.200000000000003</v>
+        <v>55.2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1569,13 +2704,13 @@
         <v>45592</v>
       </c>
       <c r="B3">
-        <v>21.25</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>21.87</v>
       </c>
       <c r="D3">
-        <v>29.4</v>
+        <v>35.49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1583,13 +2718,13 @@
         <v>45595</v>
       </c>
       <c r="B4">
-        <v>16.75</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>34.119999999999997</v>
       </c>
       <c r="D4">
-        <v>19.600000000000001</v>
+        <v>23.66</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1597,25 +2732,133 @@
         <v>45600</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>49.286999999999999</v>
       </c>
       <c r="D5">
-        <v>9.8000000000000007</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45601</v>
       </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>50.286999999999999</v>
+      </c>
       <c r="D6">
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>45587</v>
+      </c>
+      <c r="B21">
+        <v>291.2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>291.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>45595</v>
+      </c>
+      <c r="B22">
+        <f>B21-24.2</f>
+        <v>267</v>
+      </c>
+      <c r="C22">
+        <v>21.87</v>
+      </c>
+      <c r="D22">
+        <v>235.73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>45601</v>
+      </c>
+      <c r="B23">
+        <f>B22-27</f>
+        <v>240</v>
+      </c>
+      <c r="C23">
+        <v>50.286999999999999</v>
+      </c>
+      <c r="D23">
+        <v>194.13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>45608</v>
+      </c>
+      <c r="D24">
+        <v>145.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>45615</v>
+      </c>
+      <c r="D25">
+        <v>97.07</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>45622</v>
+      </c>
+      <c r="D26">
+        <v>48.53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>45629</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>